<commit_message>
cmd déplace la présentation
</commit_message>
<xml_diff>
--- a/temps de travail.xlsx
+++ b/temps de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schneider candice\OneDrive\Documents\Cours\BUT\S3\SAE302\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849C44C3-0709-4836-A089-FB4DE2912E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9257B93-4085-44C3-B5A7-ECB1E36AAC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,10 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,7 +380,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +448,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E4" si="0">(D3-C3)</f>
+        <f t="shared" ref="E3:E11" si="0">(D3-C3)</f>
         <v>0.125</v>
       </c>
       <c r="F3" s="2">
@@ -481,35 +482,118 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333331</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F11" si="1">F4+E5</f>
+        <v>0.52083333333333326</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>44895</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333331</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666652</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" s="1">
+        <v>44896</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1875</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.85416666666666652</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.85416666666666652</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.85416666666666652</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.85416666666666652</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.85416666666666652</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>